<commit_message>
Bloqueo borrar filas rhandsontable y arreglado diseño tablas editables
</commit_message>
<xml_diff>
--- a/UI/plantillas/RepGrid_Template.xlsx
+++ b/UI/plantillas/RepGrid_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stratebi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stratebi-my.sharepoint.com/personal/simonpedro_kaufmann_stratebi_com/Documents/Escritorio/GridFCM.UI/UI/plantillas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17EB7AC-9B05-44FC-9D74-AD2716973893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{979BD078-BC29-4FA9-B5B1-CEFF940D0AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22275" yWindow="-4515" windowWidth="18150" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
-  <si>
-    <t>-1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Yo - Actual</t>
   </si>
@@ -138,22 +135,24 @@
   </si>
   <si>
     <t>Constructo 10 Polo Derecho</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="72"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -171,18 +170,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,30 +248,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -503,284 +500,290 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="11" customWidth="1"/>
-    <col min="2" max="13" width="7" style="11" customWidth="1"/>
-    <col min="14" max="14" width="48.88671875" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="8.6640625" style="11"/>
+    <col min="1" max="1" width="51.54296875" style="9" customWidth="1"/>
+    <col min="2" max="13" width="11.26953125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="48.90625" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="8.6328125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="12" t="s">
-        <v>11</v>
+    </row>
+    <row r="12" spans="1:14" ht="47.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>